<commit_message>
Alterado IE-CPR para modelo "administrativo"
</commit_message>
<xml_diff>
--- a/maps/autoaprop.xlsx
+++ b/maps/autoaprop.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2064" uniqueCount="765">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2075" uniqueCount="765">
   <si>
     <t>nome_apropriador</t>
   </si>
@@ -2776,8 +2776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J380"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B28" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46:H46"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3999,6 +3999,9 @@
       <c r="H52" s="12" t="s">
         <v>4</v>
       </c>
+      <c r="J52" s="12" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="53" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
@@ -4022,6 +4025,9 @@
       <c r="H53" s="12" t="s">
         <v>4</v>
       </c>
+      <c r="J53" s="12" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="54" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
@@ -4045,6 +4051,9 @@
       <c r="H54" s="12" t="s">
         <v>4</v>
       </c>
+      <c r="J54" s="12" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="55" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
@@ -4068,6 +4077,9 @@
       <c r="H55" s="12" t="s">
         <v>4</v>
       </c>
+      <c r="J55" s="12" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="56" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
@@ -4091,6 +4103,9 @@
       <c r="H56" s="12" t="s">
         <v>4</v>
       </c>
+      <c r="J56" s="12" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="57" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
@@ -4114,6 +4129,9 @@
       <c r="H57" s="12" t="s">
         <v>4</v>
       </c>
+      <c r="J57" s="12" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="58" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
@@ -4137,6 +4155,9 @@
       <c r="H58" s="12" t="s">
         <v>4</v>
       </c>
+      <c r="J58" s="12" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="59" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
@@ -4160,6 +4181,9 @@
       <c r="H59" s="12" t="s">
         <v>4</v>
       </c>
+      <c r="J59" s="12" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="60" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="10" t="s">
@@ -4183,6 +4207,9 @@
       <c r="H60" s="12" t="s">
         <v>4</v>
       </c>
+      <c r="J60" s="12" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="61" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="10" t="s">
@@ -4206,6 +4233,9 @@
       <c r="H61" s="12" t="s">
         <v>4</v>
       </c>
+      <c r="J61" s="12" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="62" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="10" t="s">
@@ -4228,6 +4258,9 @@
       </c>
       <c r="H62" s="12" t="s">
         <v>4</v>
+      </c>
+      <c r="J62" s="12" t="s">
+        <v>743</v>
       </c>
     </row>
     <row r="63" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Atualizado IE-CEP.XLSX para modelo ADMINISTRATIVO.
</commit_message>
<xml_diff>
--- a/maps/autoaprop.xlsx
+++ b/maps/autoaprop.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2449" uniqueCount="865">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2479" uniqueCount="865">
   <si>
     <t>nome_apropriador</t>
   </si>
@@ -3077,8 +3077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J380"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A98" sqref="A98:XFD98"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3473,7 +3473,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>634</v>
       </c>
@@ -3496,7 +3496,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>616</v>
       </c>
@@ -3519,7 +3519,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>618</v>
       </c>
@@ -3542,7 +3542,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>620</v>
       </c>
@@ -3565,7 +3565,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>628</v>
       </c>
@@ -3588,7 +3588,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>499</v>
       </c>
@@ -3610,8 +3610,11 @@
       <c r="H22" s="12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J22" s="12" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>515</v>
       </c>
@@ -3633,8 +3636,11 @@
       <c r="H23" s="12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J23" s="12" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>501</v>
       </c>
@@ -3656,8 +3662,11 @@
       <c r="H24" s="12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J24" s="12" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>517</v>
       </c>
@@ -3679,8 +3688,11 @@
       <c r="H25" s="12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J25" s="12" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>503</v>
       </c>
@@ -3702,8 +3714,11 @@
       <c r="H26" s="12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J26" s="12" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>521</v>
       </c>
@@ -3725,8 +3740,11 @@
       <c r="H27" s="12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J27" s="12" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>519</v>
       </c>
@@ -3748,8 +3766,11 @@
       <c r="H28" s="12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J28" s="12" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
         <v>493</v>
       </c>
@@ -3771,8 +3792,11 @@
       <c r="H29" s="12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J29" s="12" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>523</v>
       </c>
@@ -3794,8 +3818,11 @@
       <c r="H30" s="12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J30" s="12" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
         <v>525</v>
       </c>
@@ -3817,8 +3844,11 @@
       <c r="H31" s="12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J31" s="12" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
         <v>505</v>
       </c>
@@ -3840,8 +3870,11 @@
       <c r="H32" s="12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J32" s="12" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
         <v>527</v>
       </c>
@@ -3863,8 +3896,11 @@
       <c r="H33" s="12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J33" s="12" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
         <v>529</v>
       </c>
@@ -3886,8 +3922,11 @@
       <c r="H34" s="12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J34" s="12" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
         <v>531</v>
       </c>
@@ -3909,8 +3948,11 @@
       <c r="H35" s="12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J35" s="12" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
         <v>495</v>
       </c>
@@ -3932,8 +3974,11 @@
       <c r="H36" s="12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J36" s="12" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
         <v>533</v>
       </c>
@@ -3955,8 +4000,11 @@
       <c r="H37" s="12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J37" s="12" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
         <v>497</v>
       </c>
@@ -3978,8 +4026,11 @@
       <c r="H38" s="12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J38" s="12" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
         <v>507</v>
       </c>
@@ -4001,8 +4052,11 @@
       <c r="H39" s="12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J39" s="12" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
         <v>509</v>
       </c>
@@ -4024,8 +4078,11 @@
       <c r="H40" s="12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J40" s="12" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
         <v>511</v>
       </c>
@@ -4047,8 +4104,11 @@
       <c r="H41" s="12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J41" s="12" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
         <v>513</v>
       </c>
@@ -4070,8 +4130,11 @@
       <c r="H42" s="12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J42" s="12" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
         <v>754</v>
       </c>
@@ -4093,8 +4156,11 @@
       <c r="H43" s="12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J43" s="12" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
         <v>750</v>
       </c>
@@ -4116,8 +4182,11 @@
       <c r="H44" s="12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J44" s="12" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
         <v>756</v>
       </c>
@@ -4139,8 +4208,11 @@
       <c r="H45" s="12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J45" s="12" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
         <v>752</v>
       </c>
@@ -4162,8 +4234,11 @@
       <c r="H46" s="12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J46" s="12" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
         <v>464</v>
       </c>
@@ -4185,8 +4260,11 @@
       <c r="H47" s="12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J47" s="12" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
         <v>468</v>
       </c>
@@ -4207,6 +4285,9 @@
       </c>
       <c r="H48" s="12" t="s">
         <v>4</v>
+      </c>
+      <c r="J48" s="12" t="s">
+        <v>736</v>
       </c>
     </row>
     <row r="49" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -4231,6 +4312,9 @@
       <c r="H49" s="12" t="s">
         <v>4</v>
       </c>
+      <c r="J49" s="12" t="s">
+        <v>736</v>
+      </c>
     </row>
     <row r="50" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
@@ -4254,6 +4338,9 @@
       <c r="H50" s="12" t="s">
         <v>4</v>
       </c>
+      <c r="J50" s="12" t="s">
+        <v>736</v>
+      </c>
     </row>
     <row r="51" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
@@ -4276,6 +4363,9 @@
       </c>
       <c r="H51" s="12" t="s">
         <v>4</v>
+      </c>
+      <c r="J51" s="12" t="s">
+        <v>736</v>
       </c>
     </row>
     <row r="52" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Atualizado responsável do IM_1.
</commit_message>
<xml_diff>
--- a/maps/autoaprop.xlsx
+++ b/maps/autoaprop.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2535" uniqueCount="879">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2535" uniqueCount="881">
   <si>
     <t>nome_apropriador</t>
   </si>
@@ -2692,6 +2692,12 @@
   </si>
   <si>
     <t>ARTUR LÚCIO DUARTE NETO</t>
+  </si>
+  <si>
+    <t>MARCELO MELLO MORAES</t>
+  </si>
+  <si>
+    <t>465</t>
   </si>
 </sst>
 </file>
@@ -3119,8 +3125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J386"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5536,10 +5542,10 @@
         <v>768</v>
       </c>
       <c r="D95" s="9" t="s">
-        <v>768</v>
+        <v>879</v>
       </c>
       <c r="E95" s="16" t="s">
-        <v>850</v>
+        <v>880</v>
       </c>
       <c r="F95" s="12" t="s">
         <v>130</v>
@@ -5559,10 +5565,10 @@
         <v>109</v>
       </c>
       <c r="D96" s="9" t="s">
-        <v>768</v>
+        <v>879</v>
       </c>
       <c r="E96" s="16" t="s">
-        <v>850</v>
+        <v>880</v>
       </c>
       <c r="F96" s="12" t="s">
         <v>130</v>
@@ -5582,10 +5588,10 @@
         <v>129</v>
       </c>
       <c r="D97" s="9" t="s">
-        <v>768</v>
+        <v>879</v>
       </c>
       <c r="E97" s="16" t="s">
-        <v>850</v>
+        <v>880</v>
       </c>
       <c r="F97" s="12" t="s">
         <v>130</v>
@@ -5605,10 +5611,10 @@
         <v>117</v>
       </c>
       <c r="D98" s="9" t="s">
-        <v>768</v>
+        <v>879</v>
       </c>
       <c r="E98" s="16" t="s">
-        <v>850</v>
+        <v>880</v>
       </c>
       <c r="F98" s="12" t="s">
         <v>130</v>

</xml_diff>

<commit_message>
Atualizados mapas IE-CES e IG, criado novo mapa IE.
</commit_message>
<xml_diff>
--- a/maps/autoaprop.xlsx
+++ b/maps/autoaprop.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2508" uniqueCount="874">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2508" uniqueCount="878">
   <si>
     <t>nome_apropriador</t>
   </si>
@@ -2677,6 +2677,18 @@
   </si>
   <si>
     <t>IDF_SOLDA</t>
+  </si>
+  <si>
+    <t>SETOR  IE</t>
+  </si>
+  <si>
+    <t>IE</t>
+  </si>
+  <si>
+    <t>RAFAEL F. SAMPAIO</t>
+  </si>
+  <si>
+    <t>3210</t>
   </si>
 </sst>
 </file>
@@ -3104,8 +3116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J382"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4077,62 +4089,56 @@
     </row>
     <row r="42" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
-        <v>480</v>
+        <v>846</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>481</v>
-      </c>
-      <c r="D42" s="12" t="s">
-        <v>518</v>
-      </c>
-      <c r="E42" s="12">
-        <v>3392</v>
-      </c>
-      <c r="F42" s="14" t="s">
-        <v>519</v>
+        <v>847</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>876</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>877</v>
+      </c>
+      <c r="F42" s="18" t="s">
+        <v>874</v>
       </c>
       <c r="G42" s="12" t="s">
-        <v>520</v>
+        <v>875</v>
       </c>
       <c r="H42" s="12" t="s">
         <v>4</v>
-      </c>
-      <c r="J42" s="12" t="s">
-        <v>713</v>
       </c>
     </row>
     <row r="43" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
-        <v>496</v>
+        <v>23</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>497</v>
-      </c>
-      <c r="D43" s="12" t="s">
-        <v>518</v>
-      </c>
-      <c r="E43" s="12">
-        <v>3392</v>
-      </c>
-      <c r="F43" s="14" t="s">
-        <v>519</v>
+        <v>28</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>876</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>877</v>
+      </c>
+      <c r="F43" s="18" t="s">
+        <v>874</v>
       </c>
       <c r="G43" s="12" t="s">
-        <v>520</v>
+        <v>875</v>
       </c>
       <c r="H43" s="12" t="s">
         <v>4</v>
-      </c>
-      <c r="J43" s="12" t="s">
-        <v>713</v>
       </c>
     </row>
     <row r="44" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="D44" s="12" t="s">
         <v>518</v>
@@ -4155,10 +4161,10 @@
     </row>
     <row r="45" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D45" s="12" t="s">
         <v>518</v>
@@ -4181,10 +4187,10 @@
     </row>
     <row r="46" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="D46" s="12" t="s">
         <v>518</v>
@@ -4207,10 +4213,10 @@
     </row>
     <row r="47" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="D47" s="12" t="s">
         <v>518</v>
@@ -4233,10 +4239,10 @@
     </row>
     <row r="48" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
-        <v>500</v>
+        <v>484</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>501</v>
+        <v>485</v>
       </c>
       <c r="D48" s="12" t="s">
         <v>518</v>
@@ -4259,10 +4265,10 @@
     </row>
     <row r="49" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
-        <v>474</v>
+        <v>502</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>475</v>
+        <v>503</v>
       </c>
       <c r="D49" s="12" t="s">
         <v>518</v>
@@ -4285,10 +4291,10 @@
     </row>
     <row r="50" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="D50" s="12" t="s">
         <v>518</v>
@@ -4311,10 +4317,10 @@
     </row>
     <row r="51" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
-        <v>506</v>
+        <v>474</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>507</v>
+        <v>475</v>
       </c>
       <c r="D51" s="12" t="s">
         <v>518</v>
@@ -4337,10 +4343,10 @@
     </row>
     <row r="52" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
-        <v>486</v>
+        <v>504</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>487</v>
+        <v>505</v>
       </c>
       <c r="D52" s="12" t="s">
         <v>518</v>
@@ -4363,10 +4369,10 @@
     </row>
     <row r="53" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="D53" s="12" t="s">
         <v>518</v>
@@ -4389,10 +4395,10 @@
     </row>
     <row r="54" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
-        <v>510</v>
+        <v>486</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>511</v>
+        <v>487</v>
       </c>
       <c r="D54" s="12" t="s">
         <v>518</v>
@@ -4415,10 +4421,10 @@
     </row>
     <row r="55" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="D55" s="12" t="s">
         <v>518</v>
@@ -4441,10 +4447,10 @@
     </row>
     <row r="56" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
-        <v>476</v>
+        <v>510</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>477</v>
+        <v>511</v>
       </c>
       <c r="D56" s="12" t="s">
         <v>518</v>
@@ -4467,10 +4473,10 @@
     </row>
     <row r="57" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="B57" s="11" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="D57" s="12" t="s">
         <v>518</v>
@@ -4493,10 +4499,10 @@
     </row>
     <row r="58" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="D58" s="12" t="s">
         <v>518</v>
@@ -4519,10 +4525,10 @@
     </row>
     <row r="59" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
-        <v>488</v>
+        <v>514</v>
       </c>
       <c r="B59" s="11" t="s">
-        <v>489</v>
+        <v>515</v>
       </c>
       <c r="D59" s="12" t="s">
         <v>518</v>
@@ -4545,10 +4551,10 @@
     </row>
     <row r="60" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="10" t="s">
-        <v>490</v>
+        <v>478</v>
       </c>
       <c r="B60" s="11" t="s">
-        <v>491</v>
+        <v>479</v>
       </c>
       <c r="D60" s="12" t="s">
         <v>518</v>
@@ -4571,10 +4577,10 @@
     </row>
     <row r="61" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="10" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="B61" s="11" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="D61" s="12" t="s">
         <v>518</v>
@@ -4597,10 +4603,10 @@
     </row>
     <row r="62" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="10" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="D62" s="12" t="s">
         <v>518</v>
@@ -4623,10 +4629,10 @@
     </row>
     <row r="63" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="10" t="s">
-        <v>731</v>
+        <v>492</v>
       </c>
       <c r="B63" s="11" t="s">
-        <v>732</v>
+        <v>493</v>
       </c>
       <c r="D63" s="12" t="s">
         <v>518</v>
@@ -4649,10 +4655,10 @@
     </row>
     <row r="64" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="10" t="s">
-        <v>727</v>
+        <v>494</v>
       </c>
       <c r="B64" s="11" t="s">
-        <v>728</v>
+        <v>495</v>
       </c>
       <c r="D64" s="12" t="s">
         <v>518</v>
@@ -4675,10 +4681,10 @@
     </row>
     <row r="65" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="10" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="B65" s="11" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="D65" s="12" t="s">
         <v>518</v>
@@ -4701,10 +4707,10 @@
     </row>
     <row r="66" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="10" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="D66" s="12" t="s">
         <v>518</v>
@@ -4727,22 +4733,22 @@
     </row>
     <row r="67" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="10" t="s">
-        <v>448</v>
+        <v>733</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>449</v>
+        <v>734</v>
       </c>
       <c r="D67" s="12" t="s">
-        <v>458</v>
+        <v>518</v>
       </c>
       <c r="E67" s="12">
-        <v>3170</v>
-      </c>
-      <c r="F67" s="18" t="s">
-        <v>459</v>
+        <v>3392</v>
+      </c>
+      <c r="F67" s="14" t="s">
+        <v>519</v>
       </c>
       <c r="G67" s="12" t="s">
-        <v>460</v>
+        <v>520</v>
       </c>
       <c r="H67" s="12" t="s">
         <v>4</v>
@@ -4753,22 +4759,22 @@
     </row>
     <row r="68" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="10" t="s">
-        <v>452</v>
+        <v>729</v>
       </c>
       <c r="B68" s="11" t="s">
-        <v>453</v>
+        <v>730</v>
       </c>
       <c r="D68" s="12" t="s">
-        <v>458</v>
+        <v>518</v>
       </c>
       <c r="E68" s="12">
-        <v>3170</v>
-      </c>
-      <c r="F68" s="18" t="s">
-        <v>459</v>
+        <v>3392</v>
+      </c>
+      <c r="F68" s="14" t="s">
+        <v>519</v>
       </c>
       <c r="G68" s="12" t="s">
-        <v>460</v>
+        <v>520</v>
       </c>
       <c r="H68" s="12" t="s">
         <v>4</v>
@@ -4779,10 +4785,10 @@
     </row>
     <row r="69" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="10" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B69" s="11" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D69" s="12" t="s">
         <v>458</v>
@@ -4805,10 +4811,10 @@
     </row>
     <row r="70" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="10" t="s">
-        <v>846</v>
+        <v>452</v>
       </c>
       <c r="B70" s="11" t="s">
-        <v>847</v>
+        <v>453</v>
       </c>
       <c r="D70" s="12" t="s">
         <v>458</v>
@@ -4831,10 +4837,10 @@
     </row>
     <row r="71" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="10" t="s">
-        <v>383</v>
+        <v>450</v>
       </c>
       <c r="B71" s="11" t="s">
-        <v>384</v>
+        <v>451</v>
       </c>
       <c r="D71" s="12" t="s">
         <v>458</v>
@@ -4857,10 +4863,10 @@
     </row>
     <row r="72" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="10" t="s">
-        <v>454</v>
+        <v>383</v>
       </c>
       <c r="B72" s="11" t="s">
-        <v>455</v>
+        <v>384</v>
       </c>
       <c r="D72" s="12" t="s">
         <v>458</v>
@@ -4883,10 +4889,10 @@
     </row>
     <row r="73" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="10" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B73" s="11" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="D73" s="12" t="s">
         <v>458</v>
@@ -4909,22 +4915,22 @@
     </row>
     <row r="74" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="10" t="s">
-        <v>387</v>
+        <v>456</v>
       </c>
       <c r="B74" s="11" t="s">
-        <v>388</v>
+        <v>457</v>
       </c>
       <c r="D74" s="12" t="s">
-        <v>404</v>
+        <v>458</v>
       </c>
       <c r="E74" s="12">
-        <v>3947</v>
+        <v>3170</v>
       </c>
       <c r="F74" s="18" t="s">
-        <v>409</v>
+        <v>459</v>
       </c>
       <c r="G74" s="12" t="s">
-        <v>410</v>
+        <v>460</v>
       </c>
       <c r="H74" s="12" t="s">
         <v>4</v>
@@ -4935,10 +4941,10 @@
     </row>
     <row r="75" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="10" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B75" s="11" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D75" s="12" t="s">
         <v>404</v>
@@ -4961,10 +4967,10 @@
     </row>
     <row r="76" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="10" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B76" s="11" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D76" s="12" t="s">
         <v>404</v>
@@ -4987,10 +4993,10 @@
     </row>
     <row r="77" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="10" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B77" s="11" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D77" s="12" t="s">
         <v>404</v>
@@ -5013,10 +5019,10 @@
     </row>
     <row r="78" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="10" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B78" s="11" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D78" s="12" t="s">
         <v>404</v>
@@ -5039,10 +5045,10 @@
     </row>
     <row r="79" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="10" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B79" s="11" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D79" s="12" t="s">
         <v>404</v>
@@ -5065,10 +5071,10 @@
     </row>
     <row r="80" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="10" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B80" s="11" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D80" s="12" t="s">
         <v>404</v>
@@ -5091,10 +5097,10 @@
     </row>
     <row r="81" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="10" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B81" s="11" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D81" s="12" t="s">
         <v>404</v>
@@ -5117,10 +5123,10 @@
     </row>
     <row r="82" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="10" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B82" s="11" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D82" s="12" t="s">
         <v>404</v>
@@ -5143,10 +5149,10 @@
     </row>
     <row r="83" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="10" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B83" s="11" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D83" s="12" t="s">
         <v>404</v>
@@ -5169,10 +5175,10 @@
     </row>
     <row r="84" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="10" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B84" s="11" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D84" s="12" t="s">
         <v>404</v>
@@ -5195,22 +5201,22 @@
     </row>
     <row r="85" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="10" t="s">
-        <v>665</v>
+        <v>407</v>
       </c>
       <c r="B85" s="11" t="s">
-        <v>666</v>
+        <v>408</v>
       </c>
       <c r="D85" s="12" t="s">
-        <v>672</v>
+        <v>404</v>
       </c>
       <c r="E85" s="12">
-        <v>2069</v>
-      </c>
-      <c r="F85" s="14" t="s">
-        <v>691</v>
+        <v>3947</v>
+      </c>
+      <c r="F85" s="18" t="s">
+        <v>409</v>
       </c>
       <c r="G85" s="12" t="s">
-        <v>692</v>
+        <v>410</v>
       </c>
       <c r="H85" s="12" t="s">
         <v>4</v>
@@ -5221,10 +5227,10 @@
     </row>
     <row r="86" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="10" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="B86" s="11" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="D86" s="12" t="s">
         <v>672</v>
@@ -5247,10 +5253,10 @@
     </row>
     <row r="87" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="10" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="B87" s="11" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="D87" s="12" t="s">
         <v>672</v>
@@ -5273,10 +5279,10 @@
     </row>
     <row r="88" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="10" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="B88" s="11" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="D88" s="12" t="s">
         <v>672</v>
@@ -5299,10 +5305,10 @@
     </row>
     <row r="89" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="10" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="B89" s="11" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="D89" s="12" t="s">
         <v>672</v>
@@ -5325,10 +5331,10 @@
     </row>
     <row r="90" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="10" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="B90" s="11" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="D90" s="12" t="s">
         <v>672</v>
@@ -5351,10 +5357,10 @@
     </row>
     <row r="91" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="10" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="B91" s="11" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="D91" s="12" t="s">
         <v>672</v>
@@ -5377,10 +5383,10 @@
     </row>
     <row r="92" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="10" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="B92" s="11" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="D92" s="12" t="s">
         <v>672</v>
@@ -5403,10 +5409,10 @@
     </row>
     <row r="93" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="10" t="s">
-        <v>689</v>
+        <v>679</v>
       </c>
       <c r="B93" s="11" t="s">
-        <v>690</v>
+        <v>680</v>
       </c>
       <c r="D93" s="12" t="s">
         <v>672</v>
@@ -5429,10 +5435,10 @@
     </row>
     <row r="94" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="10" t="s">
-        <v>681</v>
+        <v>689</v>
       </c>
       <c r="B94" s="11" t="s">
-        <v>682</v>
+        <v>690</v>
       </c>
       <c r="D94" s="12" t="s">
         <v>672</v>
@@ -5455,10 +5461,10 @@
     </row>
     <row r="95" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="10" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="B95" s="11" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="D95" s="12" t="s">
         <v>672</v>
@@ -5481,10 +5487,10 @@
     </row>
     <row r="96" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="10" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="B96" s="11" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="D96" s="12" t="s">
         <v>672</v>
@@ -5507,10 +5513,10 @@
     </row>
     <row r="97" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="10" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="B97" s="11" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="D97" s="12" t="s">
         <v>672</v>
@@ -5533,10 +5539,10 @@
     </row>
     <row r="98" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="10" t="s">
-        <v>858</v>
+        <v>687</v>
       </c>
       <c r="B98" s="11" t="s">
-        <v>859</v>
+        <v>688</v>
       </c>
       <c r="D98" s="12" t="s">
         <v>672</v>
@@ -5558,23 +5564,23 @@
       </c>
     </row>
     <row r="99" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B99" s="9" t="s">
-        <v>44</v>
+      <c r="A99" s="10" t="s">
+        <v>858</v>
+      </c>
+      <c r="B99" s="11" t="s">
+        <v>859</v>
       </c>
       <c r="D99" s="12" t="s">
-        <v>39</v>
+        <v>672</v>
       </c>
       <c r="E99" s="12">
-        <v>3181</v>
-      </c>
-      <c r="F99" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="G99" s="17" t="s">
-        <v>48</v>
+        <v>2069</v>
+      </c>
+      <c r="F99" s="14" t="s">
+        <v>691</v>
+      </c>
+      <c r="G99" s="12" t="s">
+        <v>692</v>
       </c>
       <c r="H99" s="12" t="s">
         <v>4</v>
@@ -5584,11 +5590,11 @@
       </c>
     </row>
     <row r="100" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B100" s="11" t="s">
-        <v>30</v>
+      <c r="A100" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B100" s="9" t="s">
+        <v>44</v>
       </c>
       <c r="D100" s="12" t="s">
         <v>39</v>
@@ -5611,10 +5617,10 @@
     </row>
     <row r="101" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="10" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B101" s="11" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D101" s="12" t="s">
         <v>39</v>
@@ -5636,11 +5642,11 @@
       </c>
     </row>
     <row r="102" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="12">
-        <v>2589</v>
-      </c>
-      <c r="B102" s="12" t="s">
-        <v>20</v>
+      <c r="A102" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B102" s="11" t="s">
+        <v>27</v>
       </c>
       <c r="D102" s="12" t="s">
         <v>39</v>
@@ -5662,11 +5668,11 @@
       </c>
     </row>
     <row r="103" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B103" s="11" t="s">
-        <v>32</v>
+      <c r="A103" s="12">
+        <v>2589</v>
+      </c>
+      <c r="B103" s="12" t="s">
+        <v>20</v>
       </c>
       <c r="D103" s="12" t="s">
         <v>39</v>
@@ -5688,11 +5694,11 @@
       </c>
     </row>
     <row r="104" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="12">
-        <v>2657</v>
-      </c>
-      <c r="B104" s="12" t="s">
-        <v>19</v>
+      <c r="A104" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B104" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="D104" s="12" t="s">
         <v>39</v>
@@ -5714,11 +5720,11 @@
       </c>
     </row>
     <row r="105" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B105" s="11" t="s">
-        <v>34</v>
+      <c r="A105" s="12">
+        <v>2657</v>
+      </c>
+      <c r="B105" s="12" t="s">
+        <v>19</v>
       </c>
       <c r="D105" s="12" t="s">
         <v>39</v>
@@ -5741,10 +5747,10 @@
     </row>
     <row r="106" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B106" s="9" t="s">
-        <v>22</v>
+        <v>33</v>
+      </c>
+      <c r="B106" s="11" t="s">
+        <v>34</v>
       </c>
       <c r="D106" s="12" t="s">
         <v>39</v>
@@ -5766,11 +5772,11 @@
       </c>
     </row>
     <row r="107" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="6" t="s">
-        <v>40</v>
+      <c r="A107" s="10" t="s">
+        <v>21</v>
       </c>
       <c r="B107" s="9" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="D107" s="12" t="s">
         <v>39</v>
@@ -5793,10 +5799,10 @@
     </row>
     <row r="108" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B108" s="9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D108" s="12" t="s">
         <v>39</v>
@@ -5819,10 +5825,10 @@
     </row>
     <row r="109" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B109" s="9" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D109" s="12" t="s">
         <v>39</v>
@@ -5844,11 +5850,11 @@
       </c>
     </row>
     <row r="110" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B110" s="15" t="s">
-        <v>25</v>
+      <c r="A110" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B110" s="9" t="s">
+        <v>46</v>
       </c>
       <c r="D110" s="12" t="s">
         <v>39</v>
@@ -5870,11 +5876,11 @@
       </c>
     </row>
     <row r="111" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B111" s="9" t="s">
-        <v>50</v>
+      <c r="A111" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B111" s="15" t="s">
+        <v>25</v>
       </c>
       <c r="D111" s="12" t="s">
         <v>39</v>
@@ -5896,11 +5902,11 @@
       </c>
     </row>
     <row r="112" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B112" s="11" t="s">
-        <v>28</v>
+      <c r="A112" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B112" s="9" t="s">
+        <v>50</v>
       </c>
       <c r="D112" s="12" t="s">
         <v>39</v>

</xml_diff>